<commit_message>
6-24-19 Latest LHC CAD Updates
</commit_message>
<xml_diff>
--- a/prj/hazelnut_large/LHC-001/1-Documentation/2019-5-22 LHC-300 Assembly Instructions/LHC-300 Sign-out Sheet.xlsx
+++ b/prj/hazelnut_large/LHC-001/1-Documentation/2019-5-22 LHC-300 Assembly Instructions/LHC-300 Sign-out Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Open AG\Documents\GitHub\openag-mechanical\prj\hazelnut_large\LHC-001\1-Documentation\2019-5-22 LHC-300 Assembly Instructions\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E6E61C7-9669-42E0-AE11-4615DAFF9B08}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E6425F93-E013-41D2-BC9A-D8801A02E1E3}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="11080" xr2:uid="{C1DC14C7-5C89-45DF-BE4F-6E1CF3C084B8}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="69">
   <si>
     <t>LHC-300 SERIAL NUMBER</t>
   </si>
@@ -228,6 +228,15 @@
   </si>
   <si>
     <t>ASSEMBLED INTO ENCLOSURE</t>
+  </si>
+  <si>
+    <t>CAPS ATTACHED</t>
+  </si>
+  <si>
+    <t>LED WIRING VERIFIED AGAIN</t>
+  </si>
+  <si>
+    <t>COMMENTS</t>
   </si>
 </sst>
 </file>
@@ -267,7 +276,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -336,21 +345,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="medium">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color indexed="64"/>
       </left>
@@ -448,6 +442,43 @@
       <right style="thin">
         <color indexed="64"/>
       </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
       <top style="thin">
         <color indexed="64"/>
       </top>
@@ -470,23 +501,20 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -495,10 +523,9 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -816,670 +843,873 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:M61"/>
+  <dimension ref="A1:I63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="A33" sqref="A33:I63"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="13.6328125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="10.6328125" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.54296875" customWidth="1"/>
-    <col min="4" max="4" width="14.90625" customWidth="1"/>
+    <col min="1" max="1" width="8.453125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="6.453125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="10.1796875" customWidth="1"/>
+    <col min="4" max="4" width="11.90625" customWidth="1"/>
     <col min="5" max="5" width="11.54296875" customWidth="1"/>
-    <col min="6" max="6" width="11.36328125" customWidth="1"/>
-    <col min="7" max="7" width="4.90625" customWidth="1"/>
-    <col min="8" max="8" width="14.54296875" customWidth="1"/>
-    <col min="9" max="9" width="10.453125" customWidth="1"/>
-    <col min="10" max="10" width="12" customWidth="1"/>
-    <col min="11" max="11" width="14" customWidth="1"/>
-    <col min="12" max="13" width="11.81640625" customWidth="1"/>
+    <col min="6" max="6" width="8.453125" customWidth="1"/>
+    <col min="7" max="7" width="10.81640625" customWidth="1"/>
+    <col min="8" max="8" width="9.90625" customWidth="1"/>
+    <col min="9" max="9" width="36.453125" customWidth="1"/>
+    <col min="10" max="10" width="10.453125" customWidth="1"/>
+    <col min="11" max="11" width="12" customWidth="1"/>
+    <col min="12" max="12" width="14" customWidth="1"/>
+    <col min="13" max="14" width="11.81640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="54.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A1" s="15" t="s">
+    <row r="1" spans="1:9" ht="55" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="14" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="15" t="s">
+      <c r="C1" s="14" t="s">
         <v>61</v>
       </c>
-      <c r="D1" s="15" t="s">
+      <c r="D1" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="E1" s="15" t="s">
+      <c r="E1" s="14" t="s">
         <v>63</v>
       </c>
-      <c r="F1" s="15" t="s">
+      <c r="F1" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="G1" s="16"/>
-      <c r="H1" s="15" t="s">
-        <v>0</v>
+      <c r="H1" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="I1" s="14" t="s">
-        <v>64</v>
-      </c>
-      <c r="J1" s="15" t="s">
-        <v>61</v>
-      </c>
-      <c r="K1" s="15" t="s">
-        <v>62</v>
-      </c>
-      <c r="L1" s="15" t="s">
-        <v>63</v>
-      </c>
-      <c r="M1" s="15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="8" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="11"/>
-      <c r="C2" s="9"/>
-      <c r="D2" s="9"/>
-      <c r="E2" s="9"/>
-      <c r="F2" s="10"/>
-      <c r="G2" s="17"/>
-      <c r="H2" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="I2" s="12"/>
-      <c r="J2" s="2"/>
-      <c r="K2" s="2"/>
-      <c r="L2" s="2"/>
-      <c r="M2" s="4"/>
-    </row>
-    <row r="3" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="B2" s="10"/>
+      <c r="C2" s="8"/>
+      <c r="D2" s="8"/>
+      <c r="E2" s="8"/>
+      <c r="F2" s="15"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+    </row>
+    <row r="3" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B3" s="12"/>
+      <c r="B3" s="11"/>
       <c r="C3" s="2"/>
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="17"/>
-      <c r="H3" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="I3" s="12"/>
-      <c r="J3" s="2"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
-      <c r="M3" s="4"/>
-    </row>
-    <row r="4" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A4" s="3" t="s">
+      <c r="F3" s="16"/>
+      <c r="G3" s="4"/>
+      <c r="H3" s="4"/>
+      <c r="I3" s="4"/>
+    </row>
+    <row r="4" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B4" s="12"/>
+      <c r="B4" s="11"/>
       <c r="C4" s="2"/>
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="17"/>
-      <c r="H4" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="I4" s="12"/>
-      <c r="J4" s="2"/>
-      <c r="K4" s="2"/>
-      <c r="L4" s="2"/>
-      <c r="M4" s="4"/>
-    </row>
-    <row r="5" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F4" s="16"/>
+      <c r="G4" s="4"/>
+      <c r="H4" s="4"/>
+      <c r="I4" s="4"/>
+    </row>
+    <row r="5" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="12"/>
+      <c r="B5" s="11"/>
       <c r="C5" s="2"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="17"/>
-      <c r="H5" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="I5" s="12"/>
-      <c r="J5" s="2"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="4"/>
-    </row>
-    <row r="6" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="F5" s="16"/>
+      <c r="G5" s="4"/>
+      <c r="H5" s="4"/>
+      <c r="I5" s="4"/>
+    </row>
+    <row r="6" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A6" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="12"/>
+      <c r="B6" s="11"/>
       <c r="C6" s="2"/>
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="17"/>
-      <c r="H6" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="I6" s="12"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="4"/>
-    </row>
-    <row r="7" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A7" s="3" t="s">
+      <c r="F6" s="16"/>
+      <c r="G6" s="4"/>
+      <c r="H6" s="4"/>
+      <c r="I6" s="4"/>
+    </row>
+    <row r="7" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A7" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="12"/>
+      <c r="B7" s="11"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="17"/>
-      <c r="H7" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="I7" s="12"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="4"/>
-    </row>
-    <row r="8" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F7" s="16"/>
+      <c r="G7" s="4"/>
+      <c r="H7" s="4"/>
+      <c r="I7" s="4"/>
+    </row>
+    <row r="8" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="12"/>
+      <c r="B8" s="11"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="17"/>
-      <c r="H8" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="I8" s="12"/>
-      <c r="J8" s="2"/>
-      <c r="K8" s="2"/>
-      <c r="L8" s="2"/>
-      <c r="M8" s="4"/>
-    </row>
-    <row r="9" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A9" s="3" t="s">
+      <c r="F8" s="16"/>
+      <c r="G8" s="4"/>
+      <c r="H8" s="4"/>
+      <c r="I8" s="4"/>
+    </row>
+    <row r="9" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="12"/>
+      <c r="B9" s="11"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="17"/>
-      <c r="H9" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="I9" s="12"/>
-      <c r="J9" s="2"/>
-      <c r="K9" s="2"/>
-      <c r="L9" s="2"/>
-      <c r="M9" s="4"/>
-    </row>
-    <row r="10" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F9" s="16"/>
+      <c r="G9" s="4"/>
+      <c r="H9" s="4"/>
+      <c r="I9" s="4"/>
+    </row>
+    <row r="10" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="12"/>
+      <c r="B10" s="11"/>
       <c r="C10" s="2"/>
       <c r="D10" s="2"/>
       <c r="E10" s="2"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="17"/>
-      <c r="H10" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="I10" s="12"/>
-      <c r="J10" s="2"/>
-      <c r="K10" s="2"/>
-      <c r="L10" s="2"/>
-      <c r="M10" s="4"/>
-    </row>
-    <row r="11" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="F10" s="16"/>
+      <c r="G10" s="4"/>
+      <c r="H10" s="4"/>
+      <c r="I10" s="4"/>
+    </row>
+    <row r="11" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A11" s="7" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="12"/>
+      <c r="B11" s="11"/>
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
       <c r="E11" s="2"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="17"/>
-      <c r="H11" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="I11" s="12"/>
-      <c r="J11" s="2"/>
-      <c r="K11" s="2"/>
-      <c r="L11" s="2"/>
-      <c r="M11" s="4"/>
-    </row>
-    <row r="12" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="F11" s="16"/>
+      <c r="G11" s="4"/>
+      <c r="H11" s="4"/>
+      <c r="I11" s="4"/>
+    </row>
+    <row r="12" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A12" s="7" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="12"/>
+      <c r="B12" s="11"/>
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
       <c r="E12" s="2"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="I12" s="12"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="4"/>
-    </row>
-    <row r="13" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F12" s="16"/>
+      <c r="G12" s="4"/>
+      <c r="H12" s="4"/>
+      <c r="I12" s="4"/>
+    </row>
+    <row r="13" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="12"/>
+      <c r="B13" s="11"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
       <c r="E13" s="2"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="17"/>
-      <c r="H13" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="I13" s="12"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="4"/>
-    </row>
-    <row r="14" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="F13" s="16"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="4"/>
+      <c r="I13" s="4"/>
+    </row>
+    <row r="14" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="7" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="12"/>
+      <c r="B14" s="11"/>
       <c r="C14" s="2"/>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="17"/>
-      <c r="H14" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="I14" s="12"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="4"/>
-    </row>
-    <row r="15" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F14" s="16"/>
+      <c r="G14" s="4"/>
+      <c r="H14" s="4"/>
+      <c r="I14" s="4"/>
+    </row>
+    <row r="15" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="12"/>
+      <c r="B15" s="11"/>
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
       <c r="E15" s="2"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="17"/>
-      <c r="H15" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="I15" s="12"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="4"/>
-    </row>
-    <row r="16" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="3" t="s">
+      <c r="F15" s="16"/>
+      <c r="G15" s="4"/>
+      <c r="H15" s="4"/>
+      <c r="I15" s="4"/>
+    </row>
+    <row r="16" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="7" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="12"/>
+      <c r="B16" s="11"/>
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
       <c r="E16" s="2"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="17"/>
-      <c r="H16" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="I16" s="12"/>
-      <c r="J16" s="2"/>
-      <c r="K16" s="2"/>
-      <c r="L16" s="2"/>
-      <c r="M16" s="4"/>
-    </row>
-    <row r="17" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="3" t="s">
+      <c r="F16" s="16"/>
+      <c r="G16" s="4"/>
+      <c r="H16" s="4"/>
+      <c r="I16" s="4"/>
+    </row>
+    <row r="17" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A17" s="7" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="12"/>
+      <c r="B17" s="11"/>
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
       <c r="E17" s="2"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="17"/>
-      <c r="H17" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="I17" s="12"/>
-      <c r="J17" s="2"/>
-      <c r="K17" s="2"/>
-      <c r="L17" s="2"/>
-      <c r="M17" s="4"/>
-    </row>
-    <row r="18" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F17" s="16"/>
+      <c r="G17" s="4"/>
+      <c r="H17" s="4"/>
+      <c r="I17" s="4"/>
+    </row>
+    <row r="18" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="12"/>
+      <c r="B18" s="11"/>
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
       <c r="E18" s="2"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="17"/>
-      <c r="H18" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="I18" s="12"/>
-      <c r="J18" s="2"/>
-      <c r="K18" s="2"/>
-      <c r="L18" s="2"/>
-      <c r="M18" s="4"/>
-    </row>
-    <row r="19" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A19" s="3" t="s">
+      <c r="F18" s="16"/>
+      <c r="G18" s="4"/>
+      <c r="H18" s="4"/>
+      <c r="I18" s="4"/>
+    </row>
+    <row r="19" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A19" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="B19" s="12"/>
+      <c r="B19" s="11"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
       <c r="E19" s="2"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="17"/>
-      <c r="H19" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="I19" s="12"/>
-      <c r="J19" s="2"/>
-      <c r="K19" s="2"/>
-      <c r="L19" s="2"/>
-      <c r="M19" s="4"/>
-    </row>
-    <row r="20" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F19" s="16"/>
+      <c r="G19" s="4"/>
+      <c r="H19" s="4"/>
+      <c r="I19" s="4"/>
+    </row>
+    <row r="20" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="B20" s="12"/>
+      <c r="B20" s="11"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
       <c r="E20" s="2"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="I20" s="12"/>
-      <c r="J20" s="2"/>
-      <c r="K20" s="2"/>
-      <c r="L20" s="2"/>
-      <c r="M20" s="4"/>
-    </row>
-    <row r="21" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A21" s="3" t="s">
+      <c r="F20" s="16"/>
+      <c r="G20" s="4"/>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4"/>
+    </row>
+    <row r="21" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A21" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="B21" s="12"/>
+      <c r="B21" s="11"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
       <c r="E21" s="2"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="17"/>
-      <c r="H21" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="I21" s="12"/>
-      <c r="J21" s="2"/>
-      <c r="K21" s="2"/>
-      <c r="L21" s="2"/>
-      <c r="M21" s="4"/>
-    </row>
-    <row r="22" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A22" s="3" t="s">
+      <c r="F21" s="16"/>
+      <c r="G21" s="4"/>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4"/>
+    </row>
+    <row r="22" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A22" s="7" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="12"/>
+      <c r="B22" s="11"/>
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
       <c r="E22" s="2"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="17"/>
-      <c r="H22" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="I22" s="12"/>
-      <c r="J22" s="2"/>
-      <c r="K22" s="2"/>
-      <c r="L22" s="2"/>
-      <c r="M22" s="4"/>
-    </row>
-    <row r="23" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F22" s="16"/>
+      <c r="G22" s="4"/>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4"/>
+    </row>
+    <row r="23" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B23" s="12"/>
+      <c r="B23" s="11"/>
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
       <c r="E23" s="2"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="17"/>
-      <c r="H23" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="I23" s="12"/>
-      <c r="J23" s="2"/>
-      <c r="K23" s="2"/>
-      <c r="L23" s="2"/>
-      <c r="M23" s="4"/>
-    </row>
-    <row r="24" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A24" s="3" t="s">
+      <c r="F23" s="16"/>
+      <c r="G23" s="4"/>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4"/>
+    </row>
+    <row r="24" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A24" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B24" s="12"/>
+      <c r="B24" s="11"/>
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
       <c r="E24" s="2"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="17"/>
-      <c r="H24" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="I24" s="12"/>
-      <c r="J24" s="2"/>
-      <c r="K24" s="2"/>
-      <c r="L24" s="2"/>
-      <c r="M24" s="4"/>
-    </row>
-    <row r="25" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F24" s="16"/>
+      <c r="G24" s="4"/>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4"/>
+    </row>
+    <row r="25" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B25" s="12"/>
+      <c r="B25" s="11"/>
       <c r="C25" s="2"/>
       <c r="D25" s="2"/>
       <c r="E25" s="2"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="17"/>
-      <c r="H25" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="I25" s="12"/>
-      <c r="J25" s="2"/>
-      <c r="K25" s="2"/>
-      <c r="L25" s="2"/>
-      <c r="M25" s="4"/>
-    </row>
-    <row r="26" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A26" s="3" t="s">
+      <c r="F25" s="16"/>
+      <c r="G25" s="4"/>
+      <c r="H25" s="4"/>
+      <c r="I25" s="4"/>
+    </row>
+    <row r="26" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A26" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B26" s="12"/>
+      <c r="B26" s="11"/>
       <c r="C26" s="2"/>
       <c r="D26" s="2"/>
       <c r="E26" s="2"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="17"/>
-      <c r="H26" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="I26" s="12"/>
-      <c r="J26" s="2"/>
-      <c r="K26" s="2"/>
-      <c r="L26" s="2"/>
-      <c r="M26" s="4"/>
-    </row>
-    <row r="27" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="3" t="s">
+      <c r="F26" s="16"/>
+      <c r="G26" s="4"/>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4"/>
+    </row>
+    <row r="27" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A27" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B27" s="12"/>
+      <c r="B27" s="11"/>
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
       <c r="E27" s="2"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="17"/>
-      <c r="H27" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="I27" s="12"/>
-      <c r="J27" s="2"/>
-      <c r="K27" s="2"/>
-      <c r="L27" s="2"/>
-      <c r="M27" s="4"/>
-    </row>
-    <row r="28" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F27" s="16"/>
+      <c r="G27" s="4"/>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4"/>
+    </row>
+    <row r="28" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B28" s="12"/>
+      <c r="B28" s="11"/>
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
       <c r="E28" s="2"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="17"/>
-      <c r="H28" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="I28" s="12"/>
-      <c r="J28" s="2"/>
-      <c r="K28" s="2"/>
-      <c r="L28" s="2"/>
-      <c r="M28" s="4"/>
-    </row>
-    <row r="29" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
-      <c r="A29" s="3" t="s">
+      <c r="F28" s="16"/>
+      <c r="G28" s="4"/>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4"/>
+    </row>
+    <row r="29" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A29" s="7" t="s">
         <v>28</v>
       </c>
-      <c r="B29" s="12"/>
+      <c r="B29" s="11"/>
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
       <c r="E29" s="2"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="17"/>
-      <c r="H29" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="I29" s="12"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="4"/>
-    </row>
-    <row r="30" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="F29" s="16"/>
+      <c r="G29" s="4"/>
+      <c r="H29" s="4"/>
+      <c r="I29" s="4"/>
+    </row>
+    <row r="30" spans="1:9" ht="19.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B30" s="12"/>
+      <c r="B30" s="11"/>
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
       <c r="E30" s="2"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="17"/>
-      <c r="H30" s="3" t="s">
+      <c r="F30" s="16"/>
+      <c r="G30" s="4"/>
+      <c r="H30" s="4"/>
+      <c r="I30" s="4"/>
+    </row>
+    <row r="31" spans="1:9" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A31" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="B31" s="12"/>
+      <c r="C31" s="5"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="17"/>
+      <c r="G31" s="6"/>
+      <c r="H31" s="6"/>
+      <c r="I31" s="6"/>
+    </row>
+    <row r="32" spans="1:9" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="33" spans="1:9" ht="61" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A33" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>61</v>
+      </c>
+      <c r="D33" s="14" t="s">
+        <v>62</v>
+      </c>
+      <c r="E33" s="14" t="s">
+        <v>63</v>
+      </c>
+      <c r="F33" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="G33" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="H33" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="I33" s="14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A34" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="B34" s="10"/>
+      <c r="C34" s="8"/>
+      <c r="D34" s="8"/>
+      <c r="E34" s="8"/>
+      <c r="F34" s="15"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+    </row>
+    <row r="35" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A35" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B35" s="11"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="16"/>
+      <c r="G35" s="4"/>
+      <c r="H35" s="4"/>
+      <c r="I35" s="4"/>
+    </row>
+    <row r="36" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A36" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="11"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="16"/>
+      <c r="G36" s="4"/>
+      <c r="H36" s="4"/>
+      <c r="I36" s="4"/>
+    </row>
+    <row r="37" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A37" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="16"/>
+      <c r="G37" s="4"/>
+      <c r="H37" s="4"/>
+      <c r="I37" s="4"/>
+    </row>
+    <row r="38" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="B38" s="11"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="16"/>
+      <c r="G38" s="4"/>
+      <c r="H38" s="4"/>
+      <c r="I38" s="4"/>
+    </row>
+    <row r="39" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A39" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B39" s="11"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="16"/>
+      <c r="G39" s="4"/>
+      <c r="H39" s="4"/>
+      <c r="I39" s="4"/>
+    </row>
+    <row r="40" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A40" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="B40" s="11"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="16"/>
+      <c r="G40" s="4"/>
+      <c r="H40" s="4"/>
+      <c r="I40" s="4"/>
+    </row>
+    <row r="41" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A41" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B41" s="11"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="16"/>
+      <c r="G41" s="4"/>
+      <c r="H41" s="4"/>
+      <c r="I41" s="4"/>
+    </row>
+    <row r="42" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A42" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="B42" s="11"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="16"/>
+      <c r="G42" s="4"/>
+      <c r="H42" s="4"/>
+      <c r="I42" s="4"/>
+    </row>
+    <row r="43" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A43" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B43" s="11"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="16"/>
+      <c r="G43" s="4"/>
+      <c r="H43" s="4"/>
+      <c r="I43" s="4"/>
+    </row>
+    <row r="44" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A44" s="7" t="s">
+        <v>41</v>
+      </c>
+      <c r="B44" s="11"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="16"/>
+      <c r="G44" s="4"/>
+      <c r="H44" s="4"/>
+      <c r="I44" s="4"/>
+    </row>
+    <row r="45" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A45" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B45" s="11"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="16"/>
+      <c r="G45" s="4"/>
+      <c r="H45" s="4"/>
+      <c r="I45" s="4"/>
+    </row>
+    <row r="46" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A46" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B46" s="11"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="16"/>
+      <c r="G46" s="4"/>
+      <c r="H46" s="4"/>
+      <c r="I46" s="4"/>
+    </row>
+    <row r="47" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A47" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B47" s="11"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="16"/>
+      <c r="G47" s="4"/>
+      <c r="H47" s="4"/>
+      <c r="I47" s="4"/>
+    </row>
+    <row r="48" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A48" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="B48" s="11"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="16"/>
+      <c r="G48" s="4"/>
+      <c r="H48" s="4"/>
+      <c r="I48" s="4"/>
+    </row>
+    <row r="49" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A49" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B49" s="11"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="16"/>
+      <c r="G49" s="4"/>
+      <c r="H49" s="4"/>
+      <c r="I49" s="4"/>
+    </row>
+    <row r="50" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A50" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="B50" s="11"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="16"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="4"/>
+      <c r="I50" s="4"/>
+    </row>
+    <row r="51" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A51" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B51" s="11"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="16"/>
+      <c r="G51" s="4"/>
+      <c r="H51" s="4"/>
+      <c r="I51" s="4"/>
+    </row>
+    <row r="52" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A52" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="B52" s="11"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="16"/>
+      <c r="G52" s="4"/>
+      <c r="H52" s="4"/>
+      <c r="I52" s="4"/>
+    </row>
+    <row r="53" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A53" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="11"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="16"/>
+      <c r="G53" s="4"/>
+      <c r="H53" s="4"/>
+      <c r="I53" s="4"/>
+    </row>
+    <row r="54" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A54" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="B54" s="11"/>
+      <c r="C54" s="2"/>
+      <c r="D54" s="2"/>
+      <c r="E54" s="2"/>
+      <c r="F54" s="16"/>
+      <c r="G54" s="4"/>
+      <c r="H54" s="4"/>
+      <c r="I54" s="4"/>
+    </row>
+    <row r="55" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A55" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B55" s="11"/>
+      <c r="C55" s="2"/>
+      <c r="D55" s="2"/>
+      <c r="E55" s="2"/>
+      <c r="F55" s="16"/>
+      <c r="G55" s="4"/>
+      <c r="H55" s="4"/>
+      <c r="I55" s="4"/>
+    </row>
+    <row r="56" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A56" s="7" t="s">
+        <v>53</v>
+      </c>
+      <c r="B56" s="11"/>
+      <c r="C56" s="2"/>
+      <c r="D56" s="2"/>
+      <c r="E56" s="2"/>
+      <c r="F56" s="16"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="4"/>
+      <c r="I56" s="4"/>
+    </row>
+    <row r="57" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A57" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B57" s="11"/>
+      <c r="C57" s="2"/>
+      <c r="D57" s="2"/>
+      <c r="E57" s="2"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="4"/>
+      <c r="I57" s="4"/>
+    </row>
+    <row r="58" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A58" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="B58" s="11"/>
+      <c r="C58" s="2"/>
+      <c r="D58" s="2"/>
+      <c r="E58" s="2"/>
+      <c r="F58" s="16"/>
+      <c r="G58" s="4"/>
+      <c r="H58" s="4"/>
+      <c r="I58" s="4"/>
+    </row>
+    <row r="59" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A59" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B59" s="11"/>
+      <c r="C59" s="2"/>
+      <c r="D59" s="2"/>
+      <c r="E59" s="2"/>
+      <c r="F59" s="16"/>
+      <c r="G59" s="4"/>
+      <c r="H59" s="4"/>
+      <c r="I59" s="4"/>
+    </row>
+    <row r="60" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A60" s="7" t="s">
+        <v>57</v>
+      </c>
+      <c r="B60" s="11"/>
+      <c r="C60" s="2"/>
+      <c r="D60" s="2"/>
+      <c r="E60" s="2"/>
+      <c r="F60" s="16"/>
+      <c r="G60" s="4"/>
+      <c r="H60" s="4"/>
+      <c r="I60" s="4"/>
+    </row>
+    <row r="61" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A61" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B61" s="11"/>
+      <c r="C61" s="2"/>
+      <c r="D61" s="2"/>
+      <c r="E61" s="2"/>
+      <c r="F61" s="16"/>
+      <c r="G61" s="4"/>
+      <c r="H61" s="4"/>
+      <c r="I61" s="4"/>
+    </row>
+    <row r="62" spans="1:9" ht="20" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A62" s="7" t="s">
         <v>59</v>
       </c>
-      <c r="I30" s="12"/>
-      <c r="J30" s="2"/>
-      <c r="K30" s="2"/>
-      <c r="L30" s="2"/>
-      <c r="M30" s="4"/>
-    </row>
-    <row r="31" spans="1:13" ht="19.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="5" t="s">
-        <v>30</v>
-      </c>
-      <c r="B31" s="13"/>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="7"/>
-      <c r="G31" s="17"/>
-      <c r="H31" s="5" t="s">
+      <c r="B62" s="11"/>
+      <c r="C62" s="2"/>
+      <c r="D62" s="2"/>
+      <c r="E62" s="2"/>
+      <c r="F62" s="16"/>
+      <c r="G62" s="4"/>
+      <c r="H62" s="4"/>
+      <c r="I62" s="4"/>
+    </row>
+    <row r="63" spans="1:9" ht="20" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A63" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="I31" s="13"/>
-      <c r="J31" s="6"/>
-      <c r="K31" s="6"/>
-      <c r="L31" s="6"/>
-      <c r="M31" s="7"/>
-    </row>
-    <row r="32" spans="1:13" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="33" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="34" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="35" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="36" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="37" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="38" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="39" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="40" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="41" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="42" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="43" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="44" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="45" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="46" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="47" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="48" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="49" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="50" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="51" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="52" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="53" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="54" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="55" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="56" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="57" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="58" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="59" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="60" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
-    <row r="61" ht="19.5" customHeight="1" x14ac:dyDescent="0.35"/>
+      <c r="B63" s="12"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="5"/>
+      <c r="E63" s="5"/>
+      <c r="F63" s="17"/>
+      <c r="G63" s="6"/>
+      <c r="H63" s="6"/>
+      <c r="I63" s="6"/>
+    </row>
   </sheetData>
-  <pageMargins left="0.25" right="0.25" top="0.25" bottom="0.25" header="0.3" footer="0.3"/>
-  <pageSetup scale="84" orientation="landscape" r:id="rId1"/>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup scale="51" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>
-    <ignoredError sqref="A2" numberStoredAsText="1"/>
+    <ignoredError sqref="A2:A3" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>